<commit_message>
All pumps working, awaits Main source control
</commit_message>
<xml_diff>
--- a/Arduino/Project 1 Arduino ini.xlsx
+++ b/Arduino/Project 1 Arduino ini.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="65">
   <si>
     <t>Serial</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Температура колектор</t>
   </si>
   <si>
-    <t>Температура отвън</t>
-  </si>
-  <si>
     <t>Комуникация</t>
   </si>
   <si>
@@ -195,16 +192,51 @@
   </si>
   <si>
     <t>Button name</t>
+  </si>
+  <si>
+    <t>3wayvalvedown</t>
+  </si>
+  <si>
+    <t>3wayValveUp</t>
+  </si>
+  <si>
+    <t>RemoteHeatPump</t>
+  </si>
+  <si>
+    <t>RemoteHeater</t>
+  </si>
+  <si>
+    <t>Температура стайна</t>
+  </si>
+  <si>
+    <t>RELAY 9</t>
+  </si>
+  <si>
+    <t>RELAY 10</t>
+  </si>
+  <si>
+    <t>RELAY 11</t>
+  </si>
+  <si>
+    <t>RELAY 12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -219,7 +251,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -227,11 +259,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -239,6 +323,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -531,7 +623,7 @@
   <dimension ref="B3:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -540,7 +632,7 @@
     <col min="3" max="3" width="8.88671875" style="1"/>
     <col min="4" max="5" width="15.88671875" style="1" customWidth="1"/>
     <col min="6" max="6" width="32" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
@@ -552,27 +644,27 @@
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>13</v>
+      <c r="F4" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
@@ -582,8 +674,8 @@
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>29</v>
+      <c r="D9" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>8</v>
@@ -599,7 +691,7 @@
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" s="9"/>
       <c r="E10" s="1" t="s">
         <v>8</v>
       </c>
@@ -614,7 +706,7 @@
       <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="9"/>
       <c r="E11" s="1" t="s">
         <v>8</v>
       </c>
@@ -629,22 +721,22 @@
       <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="9"/>
       <c r="E12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="G14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
@@ -652,19 +744,19 @@
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>27</v>
+        <v>14</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F16" t="s">
-        <v>32</v>
-      </c>
       <c r="G16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
@@ -672,17 +764,17 @@
         <v>2</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="D17" s="9"/>
       <c r="E17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F17" t="s">
-        <v>34</v>
-      </c>
       <c r="G17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
@@ -690,17 +782,17 @@
         <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="D18" s="9"/>
       <c r="E18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F18" t="s">
-        <v>36</v>
-      </c>
       <c r="G18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -708,17 +800,17 @@
         <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="D19" s="9"/>
       <c r="E19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F19" t="s">
-        <v>38</v>
-      </c>
       <c r="G19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
@@ -726,17 +818,17 @@
         <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="D20" s="9"/>
       <c r="E20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F20" t="s">
-        <v>40</v>
-      </c>
       <c r="G20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
@@ -744,17 +836,17 @@
         <v>6</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="D21" s="9"/>
       <c r="E21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F21" t="s">
-        <v>42</v>
-      </c>
       <c r="G21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
@@ -762,14 +854,17 @@
         <v>7</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="D22" s="9"/>
       <c r="E22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" t="s">
-        <v>46</v>
+        <v>42</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
@@ -777,14 +872,17 @@
         <v>8</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="D23" s="9"/>
       <c r="E23" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F23" t="s">
         <v>44</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
@@ -792,16 +890,19 @@
         <v>9</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>47</v>
+      </c>
+      <c r="G24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
@@ -809,14 +910,17 @@
         <v>10</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F25" t="s">
-        <v>48</v>
+        <v>23</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
@@ -824,11 +928,11 @@
         <v>11</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="2" t="s">
-        <v>35</v>
+        <v>24</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
@@ -836,11 +940,11 @@
         <v>12</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="2" t="s">
-        <v>37</v>
+        <v>25</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -853,5 +957,6 @@
     <mergeCell ref="D9:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>